<commit_message>
Updates to ELF and change SYVBT psg air to match Gridlab
</commit_message>
<xml_diff>
--- a/InputData/elec/ELF/Equipment Load Factors.xlsx
+++ b/InputData/elec/ELF/Equipment Load Factors.xlsx
@@ -1686,14 +1686,14 @@
         </is>
       </c>
       <c r="B2" s="12" t="n">
-        <v>2.01923</v>
+        <v>1.36302</v>
       </c>
       <c r="C2" s="12">
         <f>B2</f>
         <v/>
       </c>
       <c r="D2" s="12" t="n">
-        <v>1.06257</v>
+        <v>1.16033</v>
       </c>
     </row>
     <row r="3">
@@ -1735,14 +1735,14 @@
         </is>
       </c>
       <c r="B5" s="12" t="n">
-        <v>1.80236</v>
+        <v>1.91535</v>
       </c>
       <c r="C5" s="12">
         <f>B5</f>
         <v/>
       </c>
       <c r="D5" s="12" t="n">
-        <v>1.32205</v>
+        <v>1.45616</v>
       </c>
     </row>
     <row r="6">
@@ -1776,7 +1776,7 @@
         <v/>
       </c>
       <c r="D7" s="12" t="n">
-        <v>1.32205</v>
+        <v>1.45616</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" s="13"/>
@@ -2832,14 +2832,14 @@
         </is>
       </c>
       <c r="B3" s="12" t="n">
-        <v>22.74236</v>
+        <v>7.66676</v>
       </c>
       <c r="C3" s="12">
         <f>B3</f>
         <v/>
       </c>
       <c r="D3" s="12" t="n">
-        <v>5.753</v>
+        <v>6.54006</v>
       </c>
     </row>
     <row r="4">
@@ -2865,14 +2865,14 @@
         </is>
       </c>
       <c r="B5" s="12" t="n">
-        <v>1.74126</v>
+        <v>1.85042</v>
       </c>
       <c r="C5" s="12">
         <f>B5</f>
         <v/>
       </c>
       <c r="D5" s="12" t="n">
-        <v>1.82225</v>
+        <v>2.00709</v>
       </c>
     </row>
     <row r="6">
@@ -2906,7 +2906,7 @@
         <v/>
       </c>
       <c r="D7" s="12" t="n">
-        <v>1.82225</v>
+        <v>2.00709</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" s="13"/>
@@ -3963,10 +3963,10 @@
         </is>
       </c>
       <c r="B4" s="4" t="n">
-        <v>1.16151</v>
+        <v>1.16038</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>1.22451</v>
+        <v>1.22331</v>
       </c>
     </row>
     <row r="5">
@@ -3976,10 +3976,10 @@
         </is>
       </c>
       <c r="B5" s="4" t="n">
-        <v>1.16151</v>
+        <v>1.16038</v>
       </c>
       <c r="C5" s="4" t="n">
-        <v>1.22451</v>
+        <v>1.22331</v>
       </c>
     </row>
     <row r="6">
@@ -3989,10 +3989,10 @@
         </is>
       </c>
       <c r="B6" s="4" t="n">
-        <v>1.16151</v>
+        <v>1.16038</v>
       </c>
       <c r="C6" s="4" t="n">
-        <v>1.22451</v>
+        <v>1.22331</v>
       </c>
     </row>
     <row r="7">
@@ -4002,10 +4002,10 @@
         </is>
       </c>
       <c r="B7" s="4" t="n">
-        <v>1.16151</v>
+        <v>1.16038</v>
       </c>
       <c r="C7" s="4" t="n">
-        <v>1.22451</v>
+        <v>1.22331</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" s="13"/>

</xml_diff>

<commit_message>
Updated files from RMI
</commit_message>
<xml_diff>
--- a/InputData/elec/ELF/Equipment Load Factors.xlsx
+++ b/InputData/elec/ELF/Equipment Load Factors.xlsx
@@ -1686,14 +1686,14 @@
         </is>
       </c>
       <c r="B2" s="12" t="n">
-        <v>2.01923</v>
+        <v>1.36302</v>
       </c>
       <c r="C2" s="12">
         <f>B2</f>
         <v/>
       </c>
       <c r="D2" s="12" t="n">
-        <v>1.06257</v>
+        <v>1.16033</v>
       </c>
     </row>
     <row r="3">
@@ -1735,14 +1735,14 @@
         </is>
       </c>
       <c r="B5" s="12" t="n">
-        <v>1.80236</v>
+        <v>1.91535</v>
       </c>
       <c r="C5" s="12">
         <f>B5</f>
         <v/>
       </c>
       <c r="D5" s="12" t="n">
-        <v>1.32205</v>
+        <v>1.45616</v>
       </c>
     </row>
     <row r="6">
@@ -1776,7 +1776,7 @@
         <v/>
       </c>
       <c r="D7" s="12" t="n">
-        <v>1.32205</v>
+        <v>1.45616</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" s="13"/>
@@ -2832,14 +2832,14 @@
         </is>
       </c>
       <c r="B3" s="12" t="n">
-        <v>22.74236</v>
+        <v>7.66676</v>
       </c>
       <c r="C3" s="12">
         <f>B3</f>
         <v/>
       </c>
       <c r="D3" s="12" t="n">
-        <v>5.753</v>
+        <v>6.54006</v>
       </c>
     </row>
     <row r="4">
@@ -2865,14 +2865,14 @@
         </is>
       </c>
       <c r="B5" s="12" t="n">
-        <v>1.74126</v>
+        <v>1.85042</v>
       </c>
       <c r="C5" s="12">
         <f>B5</f>
         <v/>
       </c>
       <c r="D5" s="12" t="n">
-        <v>1.82225</v>
+        <v>2.00709</v>
       </c>
     </row>
     <row r="6">
@@ -2906,7 +2906,7 @@
         <v/>
       </c>
       <c r="D7" s="12" t="n">
-        <v>1.82225</v>
+        <v>2.00709</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" s="13"/>
@@ -3963,10 +3963,10 @@
         </is>
       </c>
       <c r="B4" s="4" t="n">
-        <v>1.16151</v>
+        <v>1.16038</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>1.22451</v>
+        <v>1.22331</v>
       </c>
     </row>
     <row r="5">
@@ -3976,10 +3976,10 @@
         </is>
       </c>
       <c r="B5" s="4" t="n">
-        <v>1.16151</v>
+        <v>1.16038</v>
       </c>
       <c r="C5" s="4" t="n">
-        <v>1.22451</v>
+        <v>1.22331</v>
       </c>
     </row>
     <row r="6">
@@ -3989,10 +3989,10 @@
         </is>
       </c>
       <c r="B6" s="4" t="n">
-        <v>1.16151</v>
+        <v>1.16038</v>
       </c>
       <c r="C6" s="4" t="n">
-        <v>1.22451</v>
+        <v>1.22331</v>
       </c>
     </row>
     <row r="7">
@@ -4002,10 +4002,10 @@
         </is>
       </c>
       <c r="B7" s="4" t="n">
-        <v>1.16151</v>
+        <v>1.16038</v>
       </c>
       <c r="C7" s="4" t="n">
-        <v>1.22451</v>
+        <v>1.22331</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" s="13"/>

</xml_diff>